<commit_message>
Updates to IOP docs
</commit_message>
<xml_diff>
--- a/MultiComp (VHDL Template)/Components/CPU/IOP16/IOP_CPU.xlsx
+++ b/MultiComp (VHDL Template)/Components/CPU/IOP16/IOP_CPU.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="104">
   <si>
     <t xml:space="preserve">INSTRUCTION</t>
   </si>
@@ -135,6 +135,15 @@
     <t xml:space="preserve">OR REG WITH IMMED VAL</t>
   </si>
   <si>
+    <t xml:space="preserve">JSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC_ADDRESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTS</t>
+  </si>
+  <si>
     <t xml:space="preserve">BEZ</t>
   </si>
   <si>
@@ -151,9 +160,6 @@
   </si>
   <si>
     <t xml:space="preserve">JMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC_ADDRESS</t>
   </si>
   <si>
     <t xml:space="preserve">JUMP TO ADDRESS</t>
@@ -464,13 +470,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="5.04"/>
@@ -783,10 +789,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>0</v>
@@ -805,28 +811,26 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -839,13 +843,11 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="R10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>1</v>
@@ -854,13 +856,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -874,16 +876,74 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="B13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -902,8 +962,18 @@
         <v>49</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
@@ -923,6 +993,8 @@
     <mergeCell ref="F9:Q9"/>
     <mergeCell ref="F10:Q10"/>
     <mergeCell ref="F11:Q11"/>
+    <mergeCell ref="F12:Q12"/>
+    <mergeCell ref="F13:Q13"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -957,24 +1029,24 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>21</v>
@@ -985,13 +1057,13 @@
         <v>24</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,13 +1071,13 @@
         <v>24</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,13 +1085,13 @@
         <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,13 +1099,13 @@
         <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,13 +1113,13 @@
         <v>24</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,13 +1127,13 @@
         <v>31</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,13 +1141,13 @@
         <v>31</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,13 +1155,13 @@
         <v>31</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,13 +1169,13 @@
         <v>31</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,30 +1183,30 @@
         <v>31</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,36 +1214,36 @@
         <v>33</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1196,7 +1268,7 @@
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.16"/>
@@ -1205,156 +1277,156 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>82</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>